<commit_message>
coding and file structure
</commit_message>
<xml_diff>
--- a/AssetSources/VoiceLines.xlsx
+++ b/AssetSources/VoiceLines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\Voice Lines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C63853-FB38-4C7D-BD0E-89DA3A053C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2171D21-8EFD-43B5-95F7-3A3B0E5CCBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="142">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -441,6 +441,27 @@
   </si>
   <si>
     <t>"Yippee! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"If you look like that, im scared to see what your parents look like."</t>
+  </si>
+  <si>
+    <t>"Its employees like you that make me happy humans are mortal!"</t>
+  </si>
+  <si>
+    <t>ParentsLookLike</t>
+  </si>
+  <si>
+    <t>MortalHumans</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>MakeYaMoreUgly</t>
+  </si>
+  <si>
+    <t>"I'll bloody make yer face even more ugly! Wait… I dinnae think that's possible."</t>
   </si>
 </sst>
 </file>
@@ -504,6 +525,20 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -517,20 +552,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -568,14 +589,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:E59" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:E59" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:E62" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -898,11 +919,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9008E0-B967-4930-8D47-663FB52657AB}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,46 +1462,40 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>127</v>
@@ -1489,12 +1504,12 @@
         <v>67</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>62</v>
@@ -1503,15 +1518,15 @@
         <v>120</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>62</v>
@@ -1520,32 +1535,29 @@
         <v>120</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>62</v>
@@ -1554,15 +1566,15 @@
         <v>120</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>62</v>
@@ -1571,15 +1583,15 @@
         <v>120</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>122</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>62</v>
@@ -1588,15 +1600,15 @@
         <v>120</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>62</v>
@@ -1605,15 +1617,15 @@
         <v>120</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>62</v>
@@ -1622,15 +1634,15 @@
         <v>120</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>62</v>
@@ -1639,15 +1651,15 @@
         <v>120</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>62</v>
@@ -1659,12 +1671,12 @@
         <v>79</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>62</v>
@@ -1676,12 +1688,12 @@
         <v>79</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>62</v>
@@ -1693,12 +1705,12 @@
         <v>79</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>62</v>
@@ -1710,12 +1722,12 @@
         <v>79</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>62</v>
@@ -1727,12 +1739,12 @@
         <v>79</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>62</v>
@@ -1744,12 +1756,12 @@
         <v>79</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>62</v>
@@ -1761,12 +1773,12 @@
         <v>79</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>62</v>
@@ -1778,12 +1790,12 @@
         <v>79</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>62</v>
@@ -1795,12 +1807,12 @@
         <v>79</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>62</v>
@@ -1812,99 +1824,150 @@
         <v>79</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>126</v>
+        <v>102</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>120</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>111</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B60 A61:B1048576 A1:B59">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="A1:B62 B63 A64:B1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Got the soft dependency for Coroner completed.
</commit_message>
<xml_diff>
--- a/AssetSources/VoiceLines.xlsx
+++ b/AssetSources/VoiceLines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2171D21-8EFD-43B5-95F7-3A3B0E5CCBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C5156A-2730-44D2-8775-D6E2AB984985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="247">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -362,24 +362,12 @@
     <t>PriorDeath</t>
   </si>
   <si>
-    <t>"a guy with a mask threw up on you and you fell over dead? maybe that possessed clone has more braincells than you!"</t>
-  </si>
-  <si>
-    <t>PriorMaskedDeath1</t>
-  </si>
-  <si>
-    <t>PriorManeaterDeath1</t>
-  </si>
-  <si>
     <t>Sniker</t>
   </si>
   <si>
     <t>Activity</t>
   </si>
   <si>
-    <t>"your parenting skills are worse than your survival skills - I didn't know that was even possible!"</t>
-  </si>
-  <si>
     <t>"You're such a bad parent, even that maneater baby wants to kill you."</t>
   </si>
   <si>
@@ -413,9 +401,6 @@
     <t>"Hello, sir Bracken! He's over there! Hahahaha"</t>
   </si>
   <si>
-    <t>PriorFall1</t>
-  </si>
-  <si>
     <t>"Remember that time you missed that jump and died? Great times."</t>
   </si>
   <si>
@@ -443,15 +428,9 @@
     <t>"Yippee! Hahahaha!"</t>
   </si>
   <si>
-    <t>"If you look like that, im scared to see what your parents look like."</t>
-  </si>
-  <si>
     <t>"Its employees like you that make me happy humans are mortal!"</t>
   </si>
   <si>
-    <t>ParentsLookLike</t>
-  </si>
-  <si>
     <t>MortalHumans</t>
   </si>
   <si>
@@ -462,6 +441,342 @@
   </si>
   <si>
     <t>"I'll bloody make yer face even more ugly! Wait… I dinnae think that's possible."</t>
+  </si>
+  <si>
+    <t>"Your parenting skills are worse than your survival skills... I dinnae know that was even possible!"</t>
+  </si>
+  <si>
+    <t>"A guy with a mask threw up on you and you fell over dead? Maybe that possessed clone has more braincells than you!"</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Bludgeoning</t>
+  </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>Blast</t>
+  </si>
+  <si>
+    <t>Strangulation</t>
+  </si>
+  <si>
+    <t>Suffocation</t>
+  </si>
+  <si>
+    <t>Mauling</t>
+  </si>
+  <si>
+    <t>Gunshots</t>
+  </si>
+  <si>
+    <t>Crushing</t>
+  </si>
+  <si>
+    <t>Drowning</t>
+  </si>
+  <si>
+    <t>Abandoned</t>
+  </si>
+  <si>
+    <t>Electrocution</t>
+  </si>
+  <si>
+    <t>Kicking</t>
+  </si>
+  <si>
+    <t>Burning</t>
+  </si>
+  <si>
+    <t>Stabbing</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>Inertia</t>
+  </si>
+  <si>
+    <t>Snipped</t>
+  </si>
+  <si>
+    <t>EnemyBaboonHawk</t>
+  </si>
+  <si>
+    <t>EnemyBracken</t>
+  </si>
+  <si>
+    <t>EnemyBunkerSpider</t>
+  </si>
+  <si>
+    <t>EnemyCircuitBees</t>
+  </si>
+  <si>
+    <t>EnemyCoilHead</t>
+  </si>
+  <si>
+    <t>EnemyEarthLeviathan</t>
+  </si>
+  <si>
+    <t>EnemyEyelessDog</t>
+  </si>
+  <si>
+    <t>EnemyGhostGirl</t>
+  </si>
+  <si>
+    <t>EnemyHoarderBug</t>
+  </si>
+  <si>
+    <t>EnemyHygrodere</t>
+  </si>
+  <si>
+    <t>EnemyJester</t>
+  </si>
+  <si>
+    <t>EnemyLassoMan</t>
+  </si>
+  <si>
+    <t>EnemySnareFlea</t>
+  </si>
+  <si>
+    <t>EnemySporeLizard</t>
+  </si>
+  <si>
+    <t>EnemyThumper</t>
+  </si>
+  <si>
+    <t>EnemyForestGiantEaten</t>
+  </si>
+  <si>
+    <t>EnemyForestGiant</t>
+  </si>
+  <si>
+    <t>EnemyMaskedPlayerWear</t>
+  </si>
+  <si>
+    <t>EnemyMaskedPlayerVictim</t>
+  </si>
+  <si>
+    <t>EnemyNutcrackerKicked</t>
+  </si>
+  <si>
+    <t>EnemyNutcrackerShot</t>
+  </si>
+  <si>
+    <t>EnemyButlerStab</t>
+  </si>
+  <si>
+    <t>EnemyButlerExplode</t>
+  </si>
+  <si>
+    <t>EnemyMaskHornets</t>
+  </si>
+  <si>
+    <t>EnemyTulipSnakeDrop</t>
+  </si>
+  <si>
+    <t>EnemyOldBirdRocket</t>
+  </si>
+  <si>
+    <t>EnemyOldBirdStomp</t>
+  </si>
+  <si>
+    <t>EnemyOldBirdCharge</t>
+  </si>
+  <si>
+    <t>EnemyOldBirdTorch</t>
+  </si>
+  <si>
+    <t>EnemyKidnapperFox</t>
+  </si>
+  <si>
+    <t>EnemyBarber</t>
+  </si>
+  <si>
+    <t>EnemyManeater</t>
+  </si>
+  <si>
+    <t>PlayerJetpackGravity</t>
+  </si>
+  <si>
+    <t>PlayerJetpackBlast</t>
+  </si>
+  <si>
+    <t>PlayerLadder</t>
+  </si>
+  <si>
+    <t>PlayerMurderShovel</t>
+  </si>
+  <si>
+    <t>PlayerMurderStopSign</t>
+  </si>
+  <si>
+    <t>PlayerMurderYieldSign</t>
+  </si>
+  <si>
+    <t>PlayerMurderKnife</t>
+  </si>
+  <si>
+    <t>PlayerEasterEgg</t>
+  </si>
+  <si>
+    <t>PlayerMurderShotgun</t>
+  </si>
+  <si>
+    <t>PlayerQuicksand</t>
+  </si>
+  <si>
+    <t>PlayerStunGrenade</t>
+  </si>
+  <si>
+    <t>PlayerCruiserDriver</t>
+  </si>
+  <si>
+    <t>PlayerCruiserPassenger</t>
+  </si>
+  <si>
+    <t>PlayerCruiserExplodeBystander</t>
+  </si>
+  <si>
+    <t>PlayerCruiserRanOver</t>
+  </si>
+  <si>
+    <t>PitGeneric</t>
+  </si>
+  <si>
+    <t>PitFacilityPit</t>
+  </si>
+  <si>
+    <t>PitFacilityCatwalkJump</t>
+  </si>
+  <si>
+    <t>PitMinePit</t>
+  </si>
+  <si>
+    <t>PitMineCave</t>
+  </si>
+  <si>
+    <t>PitMineElevator</t>
+  </si>
+  <si>
+    <t>OtherDepositItemsDesk</t>
+  </si>
+  <si>
+    <t>OtherItemDropship</t>
+  </si>
+  <si>
+    <t>OtherLandmine</t>
+  </si>
+  <si>
+    <t>OtherTurret</t>
+  </si>
+  <si>
+    <t>OtherLightning</t>
+  </si>
+  <si>
+    <t>OtherMeteor</t>
+  </si>
+  <si>
+    <t>OtherSpikeTrap</t>
+  </si>
+  <si>
+    <t>OtherOutOfBounds</t>
+  </si>
+  <si>
+    <t>EnemyLGargoyle</t>
+  </si>
+  <si>
+    <t>"You must have drawn the ugly gene in the family."</t>
+  </si>
+  <si>
+    <t>UglyGene</t>
+  </si>
+  <si>
+    <t>"I heard tough guys don't look at explosions, which is probably why you died."</t>
+  </si>
+  <si>
+    <t>"Did someone hit you with a sack of hammers?  Oh, wait, it was just a twig!  Should've seen your face!"</t>
+  </si>
+  <si>
+    <t>"What went up, came down... and splat! Just like you!"</t>
+  </si>
+  <si>
+    <t>"Gack! Couldn't breathe? Maybe you should've tried breathing through your ears!"</t>
+  </si>
+  <si>
+    <t>"Looks like someone needed a breath of fresh air...permanently!"</t>
+  </si>
+  <si>
+    <t>"Torn limb from limb?  Served you right for getting out of bed that morning!"</t>
+  </si>
+  <si>
+    <t>"Bang!  You were full of holes! What a surprise…"</t>
+  </si>
+  <si>
+    <t>"Flat as a pancake! Were you always that thin?</t>
+  </si>
+  <si>
+    <t>"You couldnae hold your breath longer than 10 seconds. Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"Left behind, eh?  Even your friends didn't like you!"</t>
+  </si>
+  <si>
+    <t>"Next to you get electrocuted, try not to pee yourself!"</t>
+  </si>
+  <si>
+    <t>"Next time you get roasted, I'll bring some marshmallows."</t>
+  </si>
+  <si>
+    <t>"Next time you see a knife, try running away from it instead of towards it! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"You got blown away, literally!"</t>
+  </si>
+  <si>
+    <t>"Next time you want to go head first into stone, I'll give ya a good smack!"</t>
+  </si>
+  <si>
+    <t>"How much glue did they need to put you back together?"</t>
+  </si>
+  <si>
+    <t>"Kicked ya right into the goal!"</t>
+  </si>
+  <si>
+    <t>"Hey employee!? How did it feel to get mauled by a BaboonHawk?"</t>
+  </si>
+  <si>
+    <t>"That Bracken really got that neck breakin'. Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"You really were a fly caught in a web! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"If you had the brains to turn around a half second sooner, you might have survived!"</t>
+  </si>
+  <si>
+    <t>"I feel sorry for that worm, you must have tasted horrible!"</t>
+  </si>
+  <si>
+    <t>"Must be pretty stupid to mess with a bees nest!"</t>
+  </si>
+  <si>
+    <t>"It's no wonder that dog ate you, it smelled your pissed pants from a mile away!"</t>
+  </si>
+  <si>
+    <t>"You couldn't even get away from a little girl! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"You got stomped by a bug! Hahahaha!"</t>
+  </si>
+  <si>
+    <t>"I can't imagine you'd be more embarrased than dying to the slowest monster on the moon."</t>
+  </si>
+  <si>
+    <t>"That jesters joke was so funny you laughed to death!"</t>
   </si>
 </sst>
 </file>
@@ -589,8 +904,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:E62" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:E62" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:E139" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:E139" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="5"/>
@@ -919,11 +1234,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9008E0-B967-4930-8D47-663FB52657AB}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +1247,7 @@
     <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -1436,7 +1751,7 @@
         <v>62</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>67</v>
@@ -1453,7 +1768,7 @@
         <v>62</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>67</v>
@@ -1464,47 +1779,50 @@
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>135</v>
+        <v>217</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>137</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,7 +1833,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>68</v>
@@ -1532,7 +1850,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>68</v>
@@ -1543,16 +1861,19 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1563,7 +1884,7 @@
         <v>62</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>73</v>
@@ -1580,7 +1901,7 @@
         <v>62</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>74</v>
@@ -1591,13 +1912,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>104</v>
@@ -1608,13 +1929,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>104</v>
@@ -1625,19 +1946,19 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>104</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1648,7 +1969,7 @@
         <v>62</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>80</v>
@@ -1659,13 +1980,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>79</v>
@@ -1676,13 +1997,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>79</v>
@@ -1693,13 +2014,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>79</v>
@@ -1716,7 +2037,7 @@
         <v>62</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>79</v>
@@ -1733,7 +2054,7 @@
         <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>79</v>
@@ -1744,13 +2065,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>79</v>
@@ -1767,7 +2088,7 @@
         <v>62</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>79</v>
@@ -1778,13 +2099,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>79</v>
@@ -1801,7 +2122,7 @@
         <v>62</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>79</v>
@@ -1818,7 +2139,7 @@
         <v>62</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>79</v>
@@ -1835,7 +2156,7 @@
         <v>62</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>79</v>
@@ -1852,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>79</v>
@@ -1869,7 +2190,7 @@
         <v>62</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>79</v>
@@ -1880,90 +2201,874 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>116</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>117</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D92" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D93" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D94" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D95" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D96" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D102" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D103" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D104" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D105" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D106" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D107" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D108" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D109" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D110" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D111" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D112" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D113" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D114" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D115" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D117" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D119" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D120" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D122" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D123" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D124" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D125" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D126" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D127" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D128" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D129" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D130" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D131" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D132" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D133" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D134" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D135" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D136" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D137" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D138" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D139" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B62 B63 A64:B1048576">
+  <conditionalFormatting sqref="A1:B82 B83 A84:B1048576">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>(INDIRECT("B"&amp;ROW()) = "X") * (MOD(ROW(),2)=1)</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs: Update README and localization files for v0.4.0
This commit updates the README and localization files to reflect the changes in version 0.4.0, including the new "PushTarget" attack pattern and related voice lines.

The following changes were made:

- Updated the README with the latest changes:
    - Separated vanilla Prior Death and Coroner Prior Death voice lines in the "Current Voice Lines" section.
    - Added Employee Classes voice lines to the "Current Voice Lines" section.
    - Included a new voice line for the gargoyle push death under "Prior Death Coroner."
- Updated the `Strings_en-us_gargoyle.xml` localization file with new death messages for the gargoyle push death.
- Changed the registry name of the gargoyle push death to avoid conflicts with the original gargoyle death registry name.
</commit_message>
<xml_diff>
--- a/AssetSources/VoiceLines.xlsx
+++ b/AssetSources/VoiceLines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149CB410-D8B1-4423-90EB-DEB5BFD19F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D378A73A-8A56-4AD6-B900-15E4717AFD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="315">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -880,12 +880,6 @@
     <t>Plague</t>
   </si>
   <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>BuiltLikeAShithouse</t>
-  </si>
-  <si>
     <t>"If yer as slow on foot as ye are in the head, ye cannae hope to hit me!"</t>
   </si>
   <si>
@@ -1024,6 +1018,15 @@
   </si>
   <si>
     <t>"Go on, then, Brute! Hit me! I could use a massage... if ye can even reach me!"</t>
+  </si>
+  <si>
+    <t>"Thought ye were safe on that catwalk? Not with him around! Hahahaha"</t>
+  </si>
+  <si>
+    <t>EnemyGargoylePush</t>
+  </si>
+  <si>
+    <t>Brute2</t>
   </si>
 </sst>
 </file>
@@ -1102,21 +1105,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1193,22 +1182,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:H146" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:H146" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}" name="Table1" displayName="Table1" ref="A1:H147" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:H147" xr:uid="{D06895C1-F989-4DBF-941D-9FC1913A8FB7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H141">
     <sortCondition ref="G1:G141"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{6266219D-B50E-4703-B88B-14976C41CFC3}" name="Redo" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{105C131E-6E82-4EC2-BC4D-862374F99D00}" name="Full file name" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{9A1DCB97-8622-4F11-A5F9-15BE399CF2EB}" name="Quote" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{3E416BA0-8256-4B96-8510-8B47E505A394}" name="Completed?" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6266219D-B50E-4703-B88B-14976C41CFC3}" name="Redo" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{486B3A15-75BF-4C98-9002-215184B9ED88}" name="Source" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A369ED74-AD6E-4F50-8F8A-A3CFB3DF9349}" name="Type" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{17C27C42-7EF0-4014-A9CB-CE0B066DC198}" name="File Name" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{105C131E-6E82-4EC2-BC4D-862374F99D00}" name="Full file name" dataDxfId="3">
       <calculatedColumnFormula>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D232A62C-0B71-4570-8881-AC19710EB804}" name="Column1" dataDxfId="4">
+    <tableColumn id="7" xr3:uid="{D232A62C-0B71-4570-8881-AC19710EB804}" name="Column1" dataDxfId="2">
       <calculatedColumnFormula>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1533,11 +1522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9008E0-B967-4930-8D47-663FB52657AB}">
-  <dimension ref="A1:H146"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1549,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>58</v>
@@ -1572,10 +1561,10 @@
         <v>17</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1777,14 +1766,14 @@
         <v>272</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>274</v>
+        <v>314</v>
       </c>
       <c r="G10" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F10</f>
-        <v>taunt_class_BuiltLikeAShithouse</v>
+        <v>taunt_employeeclass_Brute2</v>
       </c>
       <c r="H10" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
@@ -1793,7 +1782,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>62</v>
@@ -1805,7 +1794,7 @@
         <v>74</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G11" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F11</f>
@@ -1830,7 +1819,7 @@
         <v>74</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G12" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F12</f>
@@ -1843,7 +1832,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>62</v>
@@ -1855,7 +1844,7 @@
         <v>74</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G13" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F13</f>
@@ -2768,7 +2757,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>62</v>
@@ -2780,7 +2769,7 @@
         <v>67</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G50" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F50</f>
@@ -3168,7 +3157,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>62</v>
@@ -3293,7 +3282,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>62</v>
@@ -3343,7 +3332,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>62</v>
@@ -3443,7 +3432,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>62</v>
@@ -3568,7 +3557,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>62</v>
@@ -3693,7 +3682,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>62</v>
@@ -3718,7 +3707,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>62</v>
@@ -3768,7 +3757,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>62</v>
@@ -4143,7 +4132,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>62</v>
@@ -4218,7 +4207,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>62</v>
@@ -4418,7 +4407,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>62</v>
@@ -4568,7 +4557,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>62</v>
@@ -4643,7 +4632,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>62</v>
@@ -4693,7 +4682,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>62</v>
@@ -4718,7 +4707,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>62</v>
@@ -4843,7 +4832,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>62</v>
@@ -4868,7 +4857,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>62</v>
@@ -4943,7 +4932,7 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>62</v>
@@ -5068,7 +5057,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>62</v>
@@ -5077,23 +5066,23 @@
         <v>109</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="G142" s="7" t="str">
+        <v>302</v>
+      </c>
+      <c r="G142" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F142</f>
         <v>taunt_employeeclass_Scout</v>
       </c>
-      <c r="H142" s="7" t="str">
+      <c r="H142" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"A Scout? More like a... lout! Probably trip over yer own feet tryin' to escape!"&lt;/pre&gt;</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>62</v>
@@ -5102,23 +5091,23 @@
         <v>109</v>
       </c>
       <c r="E143" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F143" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F143" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="G143" s="7" t="str">
+      <c r="G143" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F143</f>
         <v>taunt_employeeclass_Brute</v>
       </c>
-      <c r="H143" s="7" t="str">
+      <c r="H143" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"Go on, then, Brute! Hit me! I could use a massage... if ye can even reach me!"&lt;/pre&gt;</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>62</v>
@@ -5127,23 +5116,23 @@
         <v>109</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="G144" s="7" t="str">
+        <v>304</v>
+      </c>
+      <c r="G144" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F144</f>
         <v>taunt_employeeclass_Researcher</v>
       </c>
-      <c r="H144" s="7" t="str">
+      <c r="H144" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"So ye think yer a smart researcher, eh? I've seen smarter rocks! And they're less squishy!"&lt;/pre&gt;</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>62</v>
@@ -5152,23 +5141,23 @@
         <v>109</v>
       </c>
       <c r="E145" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F145" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="G145" s="7" t="str">
+        <v>305</v>
+      </c>
+      <c r="G145" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F145</f>
         <v>taunt_employeeclass_Maintenance</v>
       </c>
-      <c r="H145" s="7" t="str">
+      <c r="H145" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"Go on, then, Maintenance! Try to repair yerself... after I'm done with ye!"&lt;/pre&gt;</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>62</v>
@@ -5177,18 +5166,40 @@
         <v>109</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="G146" s="7" t="str">
+        <v>306</v>
+      </c>
+      <c r="G146" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F146</f>
         <v>taunt_employeeclass_Employee</v>
       </c>
-      <c r="H146" s="7" t="str">
+      <c r="H146" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"Just a regular Employee, eh? Nothin' special... just like yer face! Hahahaha!"&lt;/pre&gt;</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G147" s="7" t="str">
+        <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F147</f>
+        <v>taunt_priordeath_EnemyGargoylePush</v>
+      </c>
+      <c r="H147" s="7" t="str">
+        <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
+        <v>&lt;pre&gt;"Thought ye were safe on that catwalk? Not with him around! Hahahaha"&lt;/pre&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(gargoyle): Add config option for "PushTarget" attack and voice line for prior death taunt
This commit adds a configuration option to enable or disable the gargoyle's new "PushTarget" attack pattern, and a dedicated voice line for dying to it.

The following changes were made:

- Added a new config option to control the "PushTarget" attack behavior.
- Disabling this option will prevent the gargoyle from using the push attack.
- Added a new voice line to the "Taunt - Prior Death/Coroner" category specifically for deaths caused by the gargoyle's push attack.
</commit_message>
<xml_diff>
--- a/AssetSources/VoiceLines.xlsx
+++ b/AssetSources/VoiceLines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Lethal Company\LethalGargoyles\AssetSources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D378A73A-8A56-4AD6-B900-15E4717AFD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3A8A42-1E80-4A79-9CBB-97500FC625CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49F33750-5E17-4167-BEC5-9ACFB1FDEA75}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="315">
   <si>
     <t>"Ach, I can smell your awful breath... all the way from here."</t>
   </si>
@@ -1078,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1096,9 +1096,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1526,7 +1523,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
+      <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5184,6 +5181,9 @@
       <c r="A147" s="1" t="s">
         <v>312</v>
       </c>
+      <c r="B147" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="D147" s="4" t="s">
         <v>109</v>
       </c>
@@ -5193,11 +5193,11 @@
       <c r="F147" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="G147" s="7" t="str">
+      <c r="G147" s="6" t="str">
         <f>"taunt_" &amp; LOWER(Table1[[#This Row],[Type]]) &amp; "_" &amp; F147</f>
         <v>taunt_priordeath_EnemyGargoylePush</v>
       </c>
-      <c r="H147" s="7" t="str">
+      <c r="H147" s="6" t="str">
         <f>"&lt;pre&gt;" &amp; Table1[[#This Row],[Quote]] &amp; IF(((Table1[[#This Row],[Source]] &lt;&gt; "Deuce") * (Table1[[#This Row],[Source]] &lt;&gt; "Fable 2"))," - Submitted by " &amp; Table1[[#This Row],[Source]],"") &amp; "&lt;/pre&gt;"</f>
         <v>&lt;pre&gt;"Thought ye were safe on that catwalk? Not with him around! Hahahaha"&lt;/pre&gt;</v>
       </c>

</xml_diff>